<commit_message>
Code commenting + tidying up.
Report essentially complete except for screenshots.

Removed a lot of console output.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,20 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27105" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27105" windowHeight="12420" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Results" sheetId="2" r:id="rId4"/>
-    <sheet name="My Results" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId6"/>
+    <sheet name="Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Analysis Empirical Recordings" sheetId="2" r:id="rId2"/>
+    <sheet name="My Implementation" sheetId="4" r:id="rId3"/>
+    <sheet name="P2P Message Headers" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="24" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
   <si>
     <t>Bandwidth</t>
   </si>
@@ -51,9 +49,6 @@
   </si>
   <si>
     <t>Predicted</t>
-  </si>
-  <si>
-    <t>iperf Tests</t>
   </si>
   <si>
     <t>Architecture</t>
@@ -131,9 +126,6 @@
     <t>P2P Chunked (Predicted)</t>
   </si>
   <si>
-    <t>My Implementation</t>
-  </si>
-  <si>
     <t>Msg Type</t>
   </si>
   <si>
@@ -174,6 +166,9 @@
   </si>
   <si>
     <t>Row Labels</t>
+  </si>
+  <si>
+    <t>iperf Tests (Averaged values from Sheet Empirical Recordings)</t>
   </si>
 </sst>
 </file>
@@ -436,55 +431,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -493,9 +449,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -521,6 +474,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,7 +575,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$6</c:f>
+              <c:f>Analysis!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -619,7 +614,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -640,7 +635,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:f>Analysis!$B$7:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -666,7 +661,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>Analysis!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -705,7 +700,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -726,7 +721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$10</c:f>
+              <c:f>Analysis!$C$7:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -752,7 +747,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>Analysis!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -791,7 +786,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -812,7 +807,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$10</c:f>
+              <c:f>Analysis!$D$7:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -838,7 +833,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$6</c:f>
+              <c:f>Analysis!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -877,7 +872,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -898,7 +893,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$10</c:f>
+              <c:f>Analysis!$E$7:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -924,7 +919,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$6</c:f>
+              <c:f>Analysis!$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -959,7 +954,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -980,7 +975,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$10</c:f>
+              <c:f>Analysis!$F$7:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1006,7 +1001,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>Analysis!$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1041,7 +1036,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1062,7 +1057,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$10</c:f>
+              <c:f>Analysis!$G$7:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1088,7 +1083,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$6</c:f>
+              <c:f>Analysis!$H$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1129,7 +1124,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>Analysis!$A$7:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1150,7 +1145,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$7:$H$10</c:f>
+              <c:f>Analysis!$H$7:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1179,11 +1174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="510781440"/>
-        <c:axId val="568578584"/>
+        <c:axId val="269460784"/>
+        <c:axId val="269459608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="510781440"/>
+        <c:axId val="269460784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1291,12 +1286,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568578584"/>
+        <c:crossAx val="269459608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="568578584"/>
+        <c:axId val="269459608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1404,7 +1399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="510781440"/>
+        <c:crossAx val="269460784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1508,14 +1503,194 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Implementation.xlsx]Sheet5!PivotTable3</c:name>
-    <c:fmtId val="11"/>
+    <c:name>[Results.xlsx]Analysis Empirical Recordings!PivotTable2</c:name>
+    <c:fmtId val="13"/>
   </c:pivotSource>
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -1526,11 +1701,23 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="1"/>
+        <c:idx val="7"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -1541,11 +1728,23 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="2"/>
+        <c:idx val="8"/>
         <c:spPr>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
@@ -1556,22 +1755,19 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="3"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -1585,11 +1781,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$B$3:$B$4</c:f>
+              <c:f>'Analysis Empirical Recordings'!$C$28:$C$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naïve Algorithm</c:v>
+                  <c:v>Test 1: Serial (UDP)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1604,13 +1800,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$8</c:f>
+              <c:f>'Analysis Empirical Recordings'!$B$30:$B$35</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1618,9 +1826,15 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>15</c:v>
                 </c:pt>
               </c:strCache>
@@ -1628,21 +1842,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$5:$B$8</c:f>
+              <c:f>'Analysis Empirical Recordings'!$C$30:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>225</c:v>
+                  <c:v>89.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>388.93333333333334</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>578.79999999999995</c:v>
+                  <c:v>448.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>784.26666666666677</c:v>
+                  <c:v>898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,11 +1868,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$C$3:$C$4</c:f>
+              <c:f>'Analysis Empirical Recordings'!$D$28:$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Random algorithm</c:v>
+                  <c:v>Test 2: Multicast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1673,13 +1887,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$8</c:f>
+              <c:f>'Analysis Empirical Recordings'!$B$30:$B$35</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1687,9 +1913,15 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>15</c:v>
                 </c:pt>
               </c:strCache>
@@ -1697,21 +1929,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$C$5:$C$8</c:f>
+              <c:f>'Analysis Empirical Recordings'!$D$30:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>181.40000000000003</c:v>
+                  <c:v>89.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>206.4</c:v>
+                  <c:v>89.799999999999983</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>238.39</c:v>
+                  <c:v>89.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>280.39999999999998</c:v>
+                  <c:v>89.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1723,11 +1961,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$D$3:$D$4</c:f>
+              <c:f>'Analysis Empirical Recordings'!$E$28:$E$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Serial (Actual)</c:v>
+                  <c:v>Test 3: Herd P2P</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1742,13 +1980,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$8</c:f>
+              <c:f>'Analysis Empirical Recordings'!$B$30:$B$35</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1756,9 +2006,15 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>15</c:v>
                 </c:pt>
               </c:strCache>
@@ -1766,79 +2022,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$D$5:$D$8</c:f>
+              <c:f>'Analysis Empirical Recordings'!$E$30:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>89.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>448.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>898</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1347</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet5!$E$3:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test 3: Herd P2P</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet5!$A$5:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet5!$E$5:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>87.223333333333343</c:v>
                 </c:pt>
@@ -1846,9 +2033,15 @@
                   <c:v>98.78</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>111.185</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>100.11500000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>114.71000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>107.23333333333335</c:v>
                 </c:pt>
               </c:numCache>
@@ -1864,12 +2057,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="523645544"/>
-        <c:axId val="523648288"/>
+        <c:axId val="267926552"/>
+        <c:axId val="437398304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="523645544"/>
+        <c:axId val="267926552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1912,7 +2106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523648288"/>
+        <c:crossAx val="437398304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1920,7 +2114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523648288"/>
+        <c:axId val="437398304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,593 +2165,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523645544"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-  </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[Implementation.xlsx]Sheet3!PivotTable2</c:name>
-    <c:fmtId val="11"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$B$3:$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test 1: Serial (UDP)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet3!$A$5:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$B$5:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>89.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>448.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>898</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1347</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test 2: Multicast</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet3!$A$5:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$C$5:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>89.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89.799999999999983</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>89.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>89.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>89.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>89.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet3!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test 3: Herd P2P</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet3!$A$5:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$D$5:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>87.223333333333343</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>98.78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111.185</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.11500000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>114.71000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>107.23333333333335</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="568578976"/>
-        <c:axId val="568578192"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="568578976"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="568578192"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="568578192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="568578976"/>
+        <c:crossAx val="267926552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2641,6 +2249,717 @@
         <c14:dropZoneFilter val="1"/>
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Results.xlsx]My Implementation!PivotTable3</c:name>
+    <c:fmtId val="15"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'My Implementation'!$B$27:$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve Algorithm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'My Implementation'!$A$29:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'My Implementation'!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>388.93333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>578.79999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>784.26666666666677</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'My Implementation'!$C$27:$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random algorithm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'My Implementation'!$A$29:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'My Implementation'!$C$29:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>181.40000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>206.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>238.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280.39999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'My Implementation'!$D$27:$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Serial (Actual)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'My Implementation'!$A$29:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'My Implementation'!$D$29:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>89.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'My Implementation'!$E$27:$E$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 3: Herd P2P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'My Implementation'!$A$29:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'My Implementation'!$E$29:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>87.223333333333343</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.11500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>107.23333333333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="446550360"/>
+        <c:axId val="446551536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="446550360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446551536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="446551536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446550360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
         <c14:dropZoneSeries val="1"/>
         <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
@@ -3286,7 +3605,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3394,11 +3713,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3409,11 +3723,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3445,9 +3754,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3802,7 +4108,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3910,6 +4216,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3920,6 +4231,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3951,6 +4267,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4343,21 +4662,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>242887</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4378,21 +4699,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4412,7 +4735,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Casey" refreshedDate="42054.804847222222" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="16">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A4:C20" sheet="Results"/>
+    <worksheetSource ref="A4:C20" sheet="Analysis Empirical Recordings"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Architecture" numFmtId="0">
@@ -4451,7 +4774,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Adam Casey" refreshedDate="42062.192655208331" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="16">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C17" sheet="My Results"/>
+    <worksheetSource ref="A1:C17" sheet="My Implementation"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Architecture" numFmtId="0">
@@ -4653,128 +4976,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
-  <location ref="A3:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Average" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="11" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="11" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12" rowHeaderCaption="Number of Nodes">
-  <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14" rowHeaderCaption="Number of Nodes">
+  <location ref="B28:E35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
       <items count="7">
@@ -4842,7 +5045,7 @@
     <dataField name="Sum of Average" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="3">
-    <chartFormat chart="11" format="0" series="1">
+    <chartFormat chart="13" format="6" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4854,7 +5057,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="11" format="1" series="1">
+    <chartFormat chart="13" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4866,7 +5069,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="11" format="2" series="1">
+    <chartFormat chart="13" format="8" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4874,6 +5077,126 @@
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="16">
+  <location ref="A27:E32" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Average" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="15" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -5153,7 +5476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -5199,45 +5522,45 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -5395,261 +5718,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5">
-        <v>225</v>
-      </c>
-      <c r="C5" s="5">
-        <v>181.40000000000003</v>
-      </c>
-      <c r="D5" s="5">
-        <v>89.8</v>
-      </c>
-      <c r="E5" s="5">
-        <v>87.223333333333343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>388.93333333333334</v>
-      </c>
-      <c r="C6" s="5">
-        <v>206.4</v>
-      </c>
-      <c r="D6" s="5">
-        <v>448.25</v>
-      </c>
-      <c r="E6" s="5">
-        <v>98.78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5">
-        <v>578.79999999999995</v>
-      </c>
-      <c r="C7" s="5">
-        <v>238.39</v>
-      </c>
-      <c r="D7" s="5">
-        <v>898</v>
-      </c>
-      <c r="E7" s="5">
-        <v>100.11500000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5">
-        <v>784.26666666666677</v>
-      </c>
-      <c r="C8" s="5">
-        <v>280.39999999999998</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1347</v>
-      </c>
-      <c r="E8" s="5">
-        <v>107.23333333333335</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D10"/>
+  <dimension ref="A4:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5">
-        <v>89.8</v>
-      </c>
-      <c r="C5" s="5">
-        <v>89.7</v>
-      </c>
-      <c r="D5" s="5">
-        <v>87.223333333333343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>448.25</v>
-      </c>
-      <c r="C6" s="5">
-        <v>89.799999999999983</v>
-      </c>
-      <c r="D6" s="5">
-        <v>98.78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5">
-        <v>89.8</v>
-      </c>
-      <c r="D7" s="5">
-        <v>111.185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>10</v>
-      </c>
-      <c r="B8" s="5">
-        <v>898</v>
-      </c>
-      <c r="C8" s="5">
-        <v>89.75</v>
-      </c>
-      <c r="D8" s="5">
-        <v>100.11500000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5">
-        <v>89.7</v>
-      </c>
-      <c r="D9" s="5">
-        <v>114.71000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1347</v>
-      </c>
-      <c r="C10" s="5">
-        <v>89.7</v>
-      </c>
-      <c r="D10" s="5">
-        <v>107.23333333333335</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:M24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C20"/>
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5662,48 +5734,48 @@
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5724,7 +5796,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -5766,7 +5838,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -5781,7 +5853,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>15</v>
@@ -5796,13 +5868,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ref="C9:C24" si="1">AVERAGE(D9:M9)</f>
+        <f t="shared" ref="C9:C20" si="1">AVERAGE(D9:M9)</f>
         <v>89.7</v>
       </c>
       <c r="D9">
@@ -5811,7 +5883,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -5850,7 +5922,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -5865,7 +5937,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -5883,7 +5955,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -5898,7 +5970,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>15</v>
@@ -5916,7 +5988,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -5937,7 +6009,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -5952,7 +6024,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -5970,7 +6042,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -5988,7 +6060,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>11</v>
@@ -6006,7 +6078,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>15</v>
@@ -6026,59 +6098,132 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>89.8</v>
+      </c>
+      <c r="D30" s="5">
+        <v>89.7</v>
+      </c>
+      <c r="E30" s="5">
+        <v>87.223333333333343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
         <v>5</v>
       </c>
-      <c r="C21" s="2">
-        <f t="shared" si="1"/>
-        <v>137.5</v>
-      </c>
-      <c r="D21">
-        <v>138.4</v>
-      </c>
-      <c r="E21">
-        <v>136.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="C31" s="5">
+        <v>448.25</v>
+      </c>
+      <c r="D31" s="5">
+        <v>89.799999999999983</v>
+      </c>
+      <c r="E31" s="5">
+        <v>98.78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>7</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5">
+        <v>89.8</v>
+      </c>
+      <c r="E32" s="5">
+        <v>111.185</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>10</v>
+      </c>
+      <c r="C33" s="5">
+        <v>898</v>
+      </c>
+      <c r="D33" s="5">
+        <v>89.75</v>
+      </c>
+      <c r="E33" s="5">
+        <v>100.11500000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>11</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5">
+        <v>89.7</v>
+      </c>
+      <c r="E34" s="5">
+        <v>114.71000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
         <v>15</v>
       </c>
-      <c r="C22" s="2">
-        <f t="shared" si="1"/>
-        <v>67.7</v>
-      </c>
-      <c r="D22">
-        <v>67.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="C35" s="5">
+        <v>1347</v>
+      </c>
+      <c r="D35" s="5">
+        <v>89.7</v>
+      </c>
+      <c r="E35" s="5">
+        <v>107.23333333333335</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6089,48 +6234,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6148,7 +6293,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -6169,7 +6314,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -6193,7 +6338,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -6214,7 +6359,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6238,7 +6383,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -6265,7 +6410,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -6289,7 +6434,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -6313,7 +6458,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6324,7 +6469,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -6335,7 +6480,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -6346,7 +6491,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>15</v>
@@ -6357,7 +6502,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6368,7 +6513,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -6379,7 +6524,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -6388,9 +6533,9 @@
         <v>100.11500000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -6399,15 +6544,109 @@
         <v>107.23333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5">
+        <v>225</v>
+      </c>
+      <c r="C29" s="5">
+        <v>181.40000000000003</v>
+      </c>
+      <c r="D29" s="5">
+        <v>89.8</v>
+      </c>
+      <c r="E29" s="5">
+        <v>87.223333333333343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>5</v>
+      </c>
+      <c r="B30" s="5">
+        <v>388.93333333333334</v>
+      </c>
+      <c r="C30" s="5">
+        <v>206.4</v>
+      </c>
+      <c r="D30" s="5">
+        <v>448.25</v>
+      </c>
+      <c r="E30" s="5">
+        <v>98.78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>10</v>
+      </c>
+      <c r="B31" s="5">
+        <v>578.79999999999995</v>
+      </c>
+      <c r="C31" s="5">
+        <v>238.39</v>
+      </c>
+      <c r="D31" s="5">
+        <v>898</v>
+      </c>
+      <c r="E31" s="5">
+        <v>100.11500000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>15</v>
+      </c>
+      <c r="B32" s="5">
+        <v>784.26666666666677</v>
+      </c>
+      <c r="C32" s="5">
+        <v>280.39999999999998</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1347</v>
+      </c>
+      <c r="E32" s="5">
+        <v>107.23333333333335</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI16"/>
   <sheetViews>
@@ -6423,510 +6662,505 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="T1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+    </row>
+    <row r="2" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8">
+        <v>15</v>
+      </c>
+      <c r="T2" s="8">
+        <v>0</v>
+      </c>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="T3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="T1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-    </row>
-    <row r="2" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9">
-        <v>15</v>
-      </c>
-      <c r="T2" s="9">
-        <v>0</v>
-      </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="33"/>
+      <c r="AE3" s="33"/>
+      <c r="AF3" s="33"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="33"/>
+    </row>
+    <row r="4" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="10" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="T4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="17"/>
+    </row>
+    <row r="5" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="T3" s="25" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="25"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="17"/>
+    </row>
+    <row r="6" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="28"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
+      <c r="AI6" s="20"/>
+    </row>
+    <row r="7" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="28"/>
+      <c r="T7" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="28" t="s">
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
+    </row>
+    <row r="8" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="31"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="21"/>
+    </row>
+    <row r="9" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="T9" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="28"/>
-    </row>
-    <row r="4" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="T4" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="31"/>
-    </row>
-    <row r="5" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="16"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="30"/>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="30"/>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="30"/>
-      <c r="AI5" s="31"/>
-    </row>
-    <row r="6" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="19"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
-      <c r="X6" s="33"/>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="33"/>
-      <c r="AA6" s="33"/>
-      <c r="AB6" s="33"/>
-      <c r="AC6" s="33"/>
-      <c r="AD6" s="33"/>
-      <c r="AE6" s="33"/>
-      <c r="AF6" s="33"/>
-      <c r="AG6" s="33"/>
-      <c r="AH6" s="33"/>
-      <c r="AI6" s="34"/>
-    </row>
-    <row r="7" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="19"/>
-      <c r="T7" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="35"/>
-      <c r="AE7" s="35"/>
-      <c r="AF7" s="35"/>
-      <c r="AG7" s="35"/>
-      <c r="AH7" s="35"/>
-      <c r="AI7" s="35"/>
-    </row>
-    <row r="8" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="22"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="35"/>
-      <c r="AE8" s="35"/>
-      <c r="AF8" s="35"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="35"/>
-      <c r="AI8" s="35"/>
-    </row>
-    <row r="9" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="T9" s="36" t="s">
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+      <c r="AH9" s="22"/>
+      <c r="AI9" s="22"/>
+    </row>
+    <row r="10" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="22"/>
+      <c r="AI10" s="22"/>
+    </row>
+    <row r="11" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="T11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="36"/>
-      <c r="AB9" s="36"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="36"/>
-      <c r="AG9" s="36"/>
-      <c r="AH9" s="36"/>
-      <c r="AI9" s="36"/>
-    </row>
-    <row r="10" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="36"/>
-      <c r="AB10" s="36"/>
-      <c r="AC10" s="36"/>
-      <c r="AD10" s="36"/>
-      <c r="AE10" s="36"/>
-      <c r="AF10" s="36"/>
-      <c r="AG10" s="36"/>
-      <c r="AH10" s="36"/>
-      <c r="AI10" s="36"/>
-    </row>
-    <row r="11" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="T11" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
-      <c r="AH11" s="14"/>
-      <c r="AI11" s="16"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="24"/>
+      <c r="AI11" s="25"/>
     </row>
     <row r="12" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T12" s="17"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="18"/>
-      <c r="AH12" s="18"/>
-      <c r="AI12" s="19"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+      <c r="AF12" s="27"/>
+      <c r="AG12" s="27"/>
+      <c r="AH12" s="27"/>
+      <c r="AI12" s="28"/>
     </row>
     <row r="13" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T13" s="17"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18"/>
-      <c r="AI13" s="19"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="27"/>
+      <c r="AB13" s="27"/>
+      <c r="AC13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="27"/>
+      <c r="AF13" s="27"/>
+      <c r="AG13" s="27"/>
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="28"/>
     </row>
     <row r="14" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T14" s="20"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
-      <c r="AE14" s="21"/>
-      <c r="AF14" s="21"/>
-      <c r="AG14" s="21"/>
-      <c r="AH14" s="21"/>
-      <c r="AI14" s="22"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AI14" s="31"/>
     </row>
     <row r="15" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-      <c r="AE15" s="23"/>
-      <c r="AF15" s="23"/>
-      <c r="AG15" s="23"/>
-      <c r="AH15" s="23"/>
-      <c r="AI15" s="23"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
     </row>
     <row r="16" spans="2:35" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="23"/>
-      <c r="AG16" s="23"/>
-      <c r="AH16" s="23"/>
-      <c r="AI16" s="23"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="T3:AA3"/>
-    <mergeCell ref="T4:AI6"/>
-    <mergeCell ref="T7:AI8"/>
-    <mergeCell ref="T9:AI10"/>
-    <mergeCell ref="T11:AI14"/>
     <mergeCell ref="B4:Q4"/>
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="B5:Q8"/>
@@ -6935,6 +7169,11 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="T3:AA3"/>
+    <mergeCell ref="T4:AI6"/>
+    <mergeCell ref="T7:AI8"/>
+    <mergeCell ref="T9:AI10"/>
+    <mergeCell ref="T11:AI14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>